<commit_message>
Generate report. deploy test 2
</commit_message>
<xml_diff>
--- a/Reports/Generated_Report.xlsx
+++ b/Reports/Generated_Report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>GRADE REPORT</t>
   </si>
@@ -20,7 +20,7 @@
     <t>Name:</t>
   </si>
   <si>
-    <t>test1</t>
+    <t>Test1</t>
   </si>
   <si>
     <t>Year:</t>
@@ -35,7 +35,7 @@
     <t>Department:</t>
   </si>
   <si>
-    <t>Electrical Engineering</t>
+    <t>Information Technology</t>
   </si>
   <si>
     <t>Units Taken:</t>
@@ -65,10 +65,10 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>NSTP 1</t>
-  </si>
-  <si>
-    <t>National Training Service Program</t>
+    <t>SEMTR</t>
+  </si>
+  <si>
+    <t>Seminars and Colloquia</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -77,76 +77,22 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>NSTP 2</t>
-  </si>
-  <si>
-    <t>National Training Service Program 2</t>
-  </si>
-  <si>
-    <t>AH 4</t>
-  </si>
-  <si>
-    <t>Reading in Visual Arts</t>
-  </si>
-  <si>
-    <t>BOSH</t>
-  </si>
-  <si>
-    <t>Basic Occupational Safety and Health</t>
-  </si>
-  <si>
-    <t>ES 5</t>
-  </si>
-  <si>
-    <t>EE 11</t>
-  </si>
-  <si>
-    <t>Electrical Circuits With Lab (DC)</t>
-  </si>
-  <si>
-    <t>EM 4 / ES 2</t>
-  </si>
-  <si>
-    <t>EE 12</t>
-  </si>
-  <si>
-    <t>Electrical Circuits: Devices and Analysis</t>
-  </si>
-  <si>
-    <t>EES 1</t>
-  </si>
-  <si>
-    <t>Fundamentals of Deformable Bodies</t>
-  </si>
-  <si>
-    <t>ES 3</t>
-  </si>
-  <si>
-    <t>EM 5</t>
-  </si>
-  <si>
-    <t>Engineering Economics</t>
-  </si>
-  <si>
-    <t>EM 1</t>
-  </si>
-  <si>
-    <t>FIL 1</t>
-  </si>
-  <si>
-    <t>Pagsasaling Wika (Teknikal)</t>
-  </si>
-  <si>
-    <t>GE 6</t>
-  </si>
-  <si>
-    <t>Art Appreciation</t>
-  </si>
-  <si>
-    <t>MST 4</t>
-  </si>
-  <si>
-    <t>Living in IT Era</t>
+    <t>ST 2</t>
+  </si>
+  <si>
+    <t>Special Topics 2 (Programming and Database)</t>
+  </si>
+  <si>
+    <t>TECHNO</t>
+  </si>
+  <si>
+    <t>Technopreneurship</t>
+  </si>
+  <si>
+    <t>TECHNO L</t>
+  </si>
+  <si>
+    <t>Technopreneurship L</t>
   </si>
 </sst>
 </file>
@@ -250,7 +196,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -315,14 +261,14 @@
         <v>8</v>
       </c>
       <c r="B4" s="11">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="11">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="12"/>
@@ -352,7 +298,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>17</v>
@@ -375,7 +321,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>21</v>
@@ -387,10 +333,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" s="13">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>20</v>
@@ -398,7 +344,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>23</v>
@@ -407,13 +353,13 @@
         <v>24</v>
       </c>
       <c r="D9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>20</v>
@@ -421,7 +367,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>25</v>
@@ -430,176 +376,15 @@
         <v>26</v>
       </c>
       <c r="D10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F10" s="13">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1">
-        <v>97</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="1">
-        <v>4</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>98</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1">
-        <v>101</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="13">
-        <v>1.75</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
-        <v>103</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <v>108</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1">
-        <v>109</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="1">
-        <v>3</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="13">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1">
-        <v>110</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="1">
-        <v>3</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="13">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>